<commit_message>
Estadistica TP2, 3, 6
</commit_message>
<xml_diff>
--- a/Estadistica/Felix - Resoluciones/Apunte 3.xlsx
+++ b/Estadistica/Felix - Resoluciones/Apunte 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9600" windowHeight="11460" firstSheet="2" activeTab="4"/>
+    <workbookView windowWidth="19200" windowHeight="11460" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
   <si>
     <t>Calcular la media de los siguientes datos: 11, 6, 7, 7, 4.</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>Q2</t>
-  </si>
-  <si>
-    <t>Ni</t>
   </si>
   <si>
     <t>Ejemplo 5. Para medir la eficacia de un método de almacenaje de harina, se sembraron 25
@@ -214,18 +211,6 @@
   </si>
   <si>
     <t>Fi-1=</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Clase Modal de 59.5-69.5</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>Marca de Clase 64,5</t>
   </si>
   <si>
     <t>fi+1 =</t>
@@ -248,7 +233,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,13 +243,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -622,7 +600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -634,9 +612,46 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -746,191 +761,239 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1269,121 +1332,121 @@
   </cols>
   <sheetData>
     <row r="1" ht="67" customHeight="1" spans="1:15">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="15" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="32" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="10">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="31">
         <v>11</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="31">
         <v>3</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="10">
+      <c r="A4" s="31">
         <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="31">
         <v>6</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="31">
         <v>5</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="10">
+      <c r="A5" s="31">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="31">
         <v>7</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="31">
         <v>2</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="31">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="10">
+      <c r="A6" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="31">
         <v>7</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="33">
         <f>SUM(J3:J5)</f>
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="10">
+      <c r="A7" s="31">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="33">
         <f>SUM(B3:B7)</f>
         <v>35</v>
       </c>
       <c r="I8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="17" cm="1">
+      <c r="J8" s="36" cm="1">
         <f t="array" ref="J8">SUM(J3:J5*I3:I5)/SUM(I3:I5)</f>
         <v>4.1</v>
       </c>
@@ -1430,269 +1493,269 @@
       </c>
     </row>
     <row r="12" ht="72" customHeight="1" spans="1:15">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="I12" s="15" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="I12" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="10">
+      <c r="A14" s="31">
         <v>1</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="31">
         <v>2</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="31">
         <v>60</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="31">
         <v>71</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="31">
         <v>80</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="31">
         <v>41</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="31">
         <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="10">
+      <c r="A15" s="31">
         <f t="shared" ref="A15:A21" si="1">A14+1</f>
         <v>2</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="31">
         <v>2</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="31">
         <v>30</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="31">
         <v>81</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="31">
         <v>41</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="31">
         <v>78</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="31">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="10">
+      <c r="A16" s="31">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="31">
         <v>3</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="31">
         <v>85</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="31">
         <v>35</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="31">
         <v>61</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="31">
         <v>55</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="31">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="10">
+      <c r="A17" s="31">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="31">
         <v>5</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="31">
         <v>52</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="31">
         <v>50</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="31">
         <v>91</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="31">
         <v>48</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="31">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="10">
+      <c r="A18" s="31">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="31">
         <v>7</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="31">
         <v>65</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="31">
         <v>35</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="31">
         <v>55</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="31">
         <v>69</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="31">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="10">
+      <c r="A19" s="31">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="31">
         <v>7</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="31">
         <v>47</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="31">
         <v>64</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="31">
         <v>73</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="31">
         <v>85</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="31">
         <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="10">
+      <c r="A20" s="31">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="31">
         <v>9</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="31">
         <v>84</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="31">
         <v>74</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="31">
         <v>59</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="31">
         <v>67</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="31">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="10">
+      <c r="A21" s="31">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="31">
         <v>10</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="31">
         <v>65</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="31">
         <v>47</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="31">
         <v>53</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="31">
         <v>39</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="31">
         <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="33">
         <f>SUM(B14:B21)</f>
         <v>45</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="31">
         <v>57</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="31">
         <v>68</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="31">
         <v>45</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="31">
         <v>76</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="31">
         <v>89</v>
       </c>
     </row>
     <row r="23" spans="9:13">
-      <c r="I23" s="10">
+      <c r="I23" s="31">
         <v>74</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="31">
         <v>54</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="31">
         <v>77</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="31">
         <v>60</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="31">
         <v>88</v>
       </c>
     </row>
@@ -1723,7 +1786,7 @@
       <c r="I25" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="38">
         <f>SUM(I14:M23)/50</f>
         <v>65.14</v>
       </c>
@@ -1760,400 +1823,430 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
+    <col min="3" max="3" width="15.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="12.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" ht="34" customHeight="1" spans="1:11">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <f>B4</f>
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <f t="shared" ref="D4:D10" si="0">B4*A4</f>
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <f>D11/B11</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" s="7">
         <f t="shared" ref="A5:A11" si="1">1+A4</f>
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <f t="shared" ref="C5:C10" si="2">B5+C4</f>
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
+      <c r="A6" s="7">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
+      <c r="A7" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="A11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="11">
         <f>SUM(B4:B10)</f>
         <v>40</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="11">
         <f>SUM(D4:D10)</f>
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+    <row r="13" ht="48" customHeight="1" spans="1:11">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" ht="19" customHeight="1" spans="1:3">
+      <c r="A14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
+      <c r="A15" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16">
+      <c r="A16" s="7">
         <v>11</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="7">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="7">
         <f>B16*A16</f>
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17">
+      <c r="A17" s="7">
         <f t="shared" ref="A17:A28" si="3">1+A16</f>
         <v>12</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="7">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="7">
         <f>B17*A17</f>
         <v>12</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="7">
         <f>C29/B29</f>
         <v>17.125</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18">
+      <c r="A18" s="7">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="7">
         <v>3</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <f t="shared" ref="C18:C28" si="4">B18*A18</f>
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19">
+      <c r="A19" s="7">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="7">
         <v>7</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <f t="shared" si="4"/>
         <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20">
+      <c r="A20" s="7">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>17</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="7">
         <f t="shared" si="4"/>
         <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21">
+      <c r="A21" s="7">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="7">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="7">
         <f t="shared" si="4"/>
         <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22">
+      <c r="A22" s="7">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="7">
         <v>15</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <f t="shared" si="4"/>
         <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23">
+      <c r="A23" s="7">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="7">
         <v>28</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="7">
         <f t="shared" si="4"/>
         <v>504</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24">
+      <c r="A24" s="7">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="7">
         <v>13</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="7">
         <f t="shared" si="4"/>
         <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25">
+      <c r="A25" s="7">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="7">
         <v>14</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="7">
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26">
+      <c r="A26" s="7">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>1</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="7">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27">
+      <c r="A27" s="7">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="7">
         <v>1</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="7">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28">
+      <c r="A28" s="7">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="11">
         <f>SUM(B16:B28)</f>
         <v>120</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="11">
         <f>SUM(C16:C28)</f>
         <v>2055</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A13:K13"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2165,634 +2258,668 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B19"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
+    <col min="1" max="1" width="10.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="10.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
     <col min="5" max="5" width="10.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" ht="33" customHeight="1" spans="1:6">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <f>B4</f>
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <f>(B7+1)/2</f>
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <f>B5+C4</f>
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <f>B6+C5</f>
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="21">
         <f>SUM(B4:B6)</f>
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row r="9" ht="33" customHeight="1" spans="1:6">
+      <c r="A9" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
+      <c r="A12" s="7">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <f>B12</f>
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <f>(B15+1)/2</f>
         <v>17.5</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1">
+      <c r="A13" s="8">
         <v>4</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="8">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="8">
         <f>B13+C12</f>
         <v>21</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <f>(4+4)/2</f>
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14">
+      <c r="A14" s="7">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>13</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="22">
         <f>B14+C13</f>
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="21">
         <f>SUM(B12:B14)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="17" ht="33" customHeight="1" spans="1:6">
+      <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="A18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20">
+      <c r="A20" s="7">
         <v>3</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>16</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="7">
         <f>B20</f>
         <v>16</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="7">
         <f>(B23+1)/2</f>
         <v>29.5</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="1">
+      <c r="A21" s="8">
         <v>4</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="8">
         <v>13</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="8">
         <f>B21+C20</f>
         <v>29</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="7">
         <f>(4+5)/2</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2">
+      <c r="A22" s="9">
         <v>5</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="9">
         <v>29</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="9">
         <f>B22+C21</f>
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="A23" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="11">
         <f>SUM(B20:B22)</f>
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+    <row r="25" ht="48" customHeight="1" spans="1:6">
+      <c r="A25" s="13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" customHeight="1" spans="1:4">
+      <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" t="s">
+      <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28">
+      <c r="A28" s="7">
         <v>1</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>9</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29">
+      <c r="A29" s="7">
         <v>2</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="7">
         <v>6</v>
       </c>
-      <c r="C29">
-        <f>B29+C28</f>
+      <c r="C29" s="7">
+        <f t="shared" ref="C29:C34" si="0">B29+C28</f>
         <v>15</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="7">
         <f>(B35+1)/2</f>
         <v>20.5</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="1">
+      <c r="A30" s="8">
         <v>3</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="8">
         <v>10</v>
       </c>
-      <c r="C30" s="1">
-        <f>B30+C29</f>
+      <c r="C30" s="8">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" s="23"/>
+      <c r="E30" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="7">
         <f>(3+3)/2</f>
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31">
+      <c r="A31" s="7">
         <v>4</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="7">
         <v>10</v>
       </c>
-      <c r="C31">
-        <f>B31+C30</f>
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32">
+      <c r="A32" s="7">
         <v>5</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="7">
         <v>3</v>
       </c>
-      <c r="C32">
-        <f>B32+C31</f>
+      <c r="C32" s="7">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33">
+      <c r="A33" s="7">
         <v>6</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="7">
         <v>1</v>
       </c>
-      <c r="C33">
-        <f>B33+C32</f>
+      <c r="C33" s="7">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34">
+      <c r="A34" s="7">
         <v>8</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="7">
         <v>1</v>
       </c>
-      <c r="C34">
-        <f>B34+C33</f>
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="A35" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="11">
         <f>SUM(B28:B34)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" t="s">
+      <c r="A39" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40">
+      <c r="A40" s="7">
         <v>11</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="7">
         <v>1</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41">
+      <c r="A41" s="7">
         <f>A40+1</f>
         <v>12</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="7">
         <v>1</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="7">
         <f>B41+C40</f>
         <v>2</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="7">
         <f>(B53+1)/2</f>
         <v>60.5</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42">
-        <f t="shared" ref="A42:A48" si="0">A41+1</f>
+      <c r="A42" s="7">
+        <f t="shared" ref="A42:A52" si="1">A41+1</f>
         <v>13</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="7">
         <v>3</v>
       </c>
-      <c r="C42">
-        <f t="shared" ref="C42:C52" si="1">B42+C41</f>
+      <c r="C42" s="7">
+        <f t="shared" ref="C42:C52" si="2">B42+C41</f>
         <v>5</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="7">
         <f>(15+15)/2</f>
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43">
-        <f t="shared" si="0"/>
+      <c r="A43" s="7">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="7">
         <v>7</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="7">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="7">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="7">
         <v>17</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="7">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="7">
         <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="7">
         <v>18</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="7">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="8">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="8">
         <v>15</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="8">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="7">
         <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="7">
         <v>28</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="7">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="7">
         <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="7">
         <v>13</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="7">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="7">
         <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49">
-        <f>A48+1</f>
         <v>20</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="7">
         <v>14</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="7">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="7">
         <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50">
-        <f>A49+1</f>
         <v>21</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="7">
         <v>1</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="7">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="7">
         <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51">
-        <f>A50+1</f>
         <v>22</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="7">
         <v>1</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="7">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="7">
         <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
-        <f>A51+1</f>
         <v>23</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="7">
         <v>1</v>
       </c>
-      <c r="C52">
-        <f t="shared" si="1"/>
+      <c r="C52" s="7">
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="A53" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="11">
         <f>SUM(B40:B52)</f>
         <v>120</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A37:F37"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2801,193 +2928,218 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="31.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" ht="31" customHeight="1" spans="1:7">
+      <c r="A1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" s="7">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B7" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="B9" s="11">
         <f>SUM(B4:B8)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
+    <row r="11" ht="36" customHeight="1" spans="1:7">
+      <c r="A11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14">
+      <c r="A14" s="15">
         <v>1</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
+    <row r="15" spans="1:7">
+      <c r="A15" s="15">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E15" cm="1">
+      <c r="E15" s="17" cm="1">
         <f t="array" ref="E15">MODE(B14:B20)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1">
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="20">
         <v>3</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="8">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
+      <c r="E16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="1">
+      <c r="A17" s="20">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18">
+      <c r="A18" s="15">
         <v>5</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19">
+      <c r="A19" s="15">
         <v>6</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20">
+      <c r="A20" s="15">
         <v>8</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="A21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="11">
         <f>SUM(B14:B20)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2996,411 +3148,414 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.85714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.8571428571429"/>
-    <col min="4" max="4" width="10.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="12.8571428571429"/>
+    <col min="1" max="1" width="15.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="13.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="9.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="14.7142857142857" customWidth="1"/>
+    <col min="5" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="15.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" ht="39" customHeight="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" ht="24" customHeight="1" spans="1:7">
+      <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="A4" s="7">
         <v>29.5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>39.5</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C6" si="0">_xlfn.CONCAT(A4," - ",B4)</f>
+      <c r="C4" s="7" t="str">
+        <f t="shared" ref="C4:C10" si="0">_xlfn.CONCAT(A4," - ",B4)</f>
         <v>29,5 - 39,5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <f>(B4+A4)/2</f>
         <v>34.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <f>E4*D4</f>
         <v>138</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <f>E4</f>
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5">
+      <c r="A5" s="7">
         <f>B4</f>
         <v>39.5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7">
         <f>B4+10</f>
         <v>49.5</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>39,5 - 49,5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <f t="shared" ref="D5:D10" si="1">(B5+A5)/2</f>
         <v>44.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="7">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <f t="shared" ref="F5:F10" si="2">E5*D5</f>
         <v>267</v>
       </c>
-      <c r="G5">
-        <f>E5+G4</f>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G10" si="3">E5+G4</f>
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6">
-        <f t="shared" ref="A6:A11" si="3">B5</f>
+      <c r="A6" s="7">
+        <f t="shared" ref="A6:A11" si="4">B5</f>
         <v>49.5</v>
       </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B11" si="4">B5+10</f>
+      <c r="B6" s="7">
+        <f t="shared" ref="B6:B11" si="5">B5+10</f>
         <v>59.5</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>49,5 - 59,5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <f t="shared" si="1"/>
         <v>54.5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="7">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7">
         <f t="shared" si="2"/>
         <v>436</v>
       </c>
-      <c r="G6">
-        <f>E6+G5</f>
+      <c r="G6" s="7">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1">
+      <c r="A7" s="8">
+        <f t="shared" si="4"/>
+        <v>59.5</v>
+      </c>
+      <c r="B7" s="8">
+        <f t="shared" si="5"/>
+        <v>69.5</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>59,5 - 69,5</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>12</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>774</v>
+      </c>
+      <c r="G7" s="8">
         <f t="shared" si="3"/>
-        <v>59.5</v>
-      </c>
-      <c r="B7" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="7">
         <f t="shared" si="4"/>
         <v>69.5</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f>_xlfn.CONCAT(A7," - ",B7)</f>
-        <v>59,5 - 69,5</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="B8" s="7">
+        <f t="shared" si="5"/>
+        <v>79.5</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>69,5 - 79,5</v>
+      </c>
+      <c r="D8" s="7">
         <f t="shared" si="1"/>
-        <v>64.5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+        <v>74.5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>9</v>
+      </c>
+      <c r="F8" s="7">
         <f t="shared" si="2"/>
-        <v>774</v>
-      </c>
-      <c r="G7" s="1">
-        <f>E7+G6</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
+        <v>670.5</v>
+      </c>
+      <c r="G8" s="7">
         <f t="shared" si="3"/>
-        <v>69.5</v>
-      </c>
-      <c r="B8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="7">
         <f t="shared" si="4"/>
         <v>79.5</v>
       </c>
-      <c r="C8" t="str">
-        <f>_xlfn.CONCAT(A8," - ",B8)</f>
-        <v>69,5 - 79,5</v>
-      </c>
-      <c r="D8">
+      <c r="B9" s="7">
+        <f t="shared" si="5"/>
+        <v>89.5</v>
+      </c>
+      <c r="C9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>79,5 - 89,5</v>
+      </c>
+      <c r="D9" s="7">
         <f t="shared" si="1"/>
-        <v>74.5</v>
-      </c>
-      <c r="E8">
-        <v>9</v>
-      </c>
-      <c r="F8">
+        <v>84.5</v>
+      </c>
+      <c r="E9" s="7">
+        <v>7</v>
+      </c>
+      <c r="F9" s="7">
         <f t="shared" si="2"/>
-        <v>670.5</v>
-      </c>
-      <c r="G8">
-        <f>E8+G7</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
+        <v>591.5</v>
+      </c>
+      <c r="G9" s="7">
         <f t="shared" si="3"/>
-        <v>79.5</v>
-      </c>
-      <c r="B9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="7">
         <f t="shared" si="4"/>
         <v>89.5</v>
       </c>
-      <c r="C9" t="str">
-        <f>_xlfn.CONCAT(A9," - ",B9)</f>
-        <v>79,5 - 89,5</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>84.5</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>591.5</v>
-      </c>
-      <c r="G9">
-        <f>E9+G8</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <f t="shared" si="3"/>
-        <v>89.5</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="4"/>
+      <c r="B10" s="7">
+        <f t="shared" si="5"/>
         <v>99.5</v>
       </c>
-      <c r="C10" t="str">
-        <f>_xlfn.CONCAT(A10," - ",B10)</f>
+      <c r="C10" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>89,5 - 99,5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <f t="shared" si="1"/>
         <v>94.5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="7">
         <f t="shared" si="2"/>
         <v>378</v>
       </c>
-      <c r="G10">
-        <f>E10+G9</f>
+      <c r="G10" s="7">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="4:6">
-      <c r="D11" t="s">
+      <c r="D11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="11">
         <f>SUM(E4:E10)</f>
         <v>50</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="11">
         <f>SUM(F4:F10)</f>
         <v>3255</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="7">
         <f>F11/E11</f>
         <v>65.1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="7">
         <f>(E11+1)/2</f>
         <v>25.5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <f>E17*(B17-B18)/E16+B16</f>
         <v>65.3333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="4"/>
+      <c r="A15" s="12"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="7">
         <f>A7</f>
         <v>59.5</v>
       </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16">
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="7">
         <f>E7</f>
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="7">
         <f>E11/2</f>
         <v>25</v>
       </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17">
+      <c r="D17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="7">
         <f>B7-A7</f>
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="7">
         <f>G6</f>
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <f>B22+E23*(B23-B24)/(B23-B24+B23-E22)</f>
         <v>65.2142857142857</v>
       </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="7">
         <f>A7</f>
         <v>59.5</v>
       </c>
-      <c r="D22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="7">
         <f>E8</f>
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="7">
         <f>E7</f>
         <v>12</v>
       </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="7">
         <f>B7-A7</f>
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="7">
         <f>E6</f>
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>